<commit_message>
Adicionei o backlog da sprint 2
</commit_message>
<xml_diff>
--- a/Documentação/Product BackLog/Product Backlog.xlsx
+++ b/Documentação/Product BackLog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatec\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/162b3d46c84f4e18/Documentos/LILIAN/FATEC/API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B72D924-E1ED-4B2C-B598-78BB69C7133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A470B00A-65FE-4EF2-8AA6-CCB46402327F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{ADB6CCF0-5F3A-47F8-B312-800F15360062}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADB6CCF0-5F3A-47F8-B312-800F15360062}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Sprint</t>
   </si>
@@ -142,13 +142,6 @@
   </si>
   <si>
     <t>Raspagem de dados das informações sobre a COVID-19 do DataSUS TABNET das cidades de Taubaté, Jacareí e São José dos Campos</t>
-  </si>
-  <si>
-    <t>Criação e organização das tabelas de dados por contaminação,
-  internação e óbitos dos anos de 2019 a 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criação da página HOME </t>
   </si>
   <si>
     <t xml:space="preserve">Implementação das tabelas obtidas na página Web </t>
@@ -208,13 +201,35 @@
   </si>
   <si>
     <t>Integração final do projeto no repositório GIT</t>
+  </si>
+  <si>
+    <t>Criação da página " Dados da Covid"</t>
+  </si>
+  <si>
+    <t>Criação da página "Conheça o Projeto"</t>
+  </si>
+  <si>
+    <t>Criação da página "HOME"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Criação e organização das tabelas de dados por contaminação,
+ internação e óbitos dos anos de 2019 a 2022</t>
+  </si>
+  <si>
+    <t>Lilian e Douglas</t>
+  </si>
+  <si>
+    <t>Katiane e Gabriela</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,6 +350,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -671,23 +690,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F0D08F-C38B-40B3-B766-4D2804EBD28B}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -707,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -719,7 +738,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -737,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -755,7 +774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -773,7 +792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45.75">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -785,7 +804,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -803,7 +822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30.75">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>1</v>
       </c>
@@ -816,7 +835,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -834,7 +853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -852,7 +871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -870,7 +889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -888,7 +907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -906,7 +925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -924,7 +943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>2</v>
       </c>
@@ -933,58 +952,85 @@
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:7" ht="30.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="30.75">
+      <c r="D16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="D17" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="D18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="D19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -992,237 +1038,267 @@
         <v>32</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="30">
+      <c r="D20" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>3</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" ht="30.75">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="B22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>3</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="12">
+      <c r="B23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>3</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" ht="45">
+      <c r="B24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>3</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="30">
-      <c r="A26" s="3">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
         <v>3</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="45">
+      <c r="B26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>3</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>3</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>3</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="45">
-      <c r="A30" s="12">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>3</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
         <v>4</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="1:6" ht="45.75">
-      <c r="A31" s="3">
-        <v>4</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" ht="30.75">
-      <c r="A32" s="3">
-        <v>4</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="B32" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>4</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>4</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="60">
-      <c r="A35" s="12">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>4</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="1:6" ht="60">
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>4</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" ht="60">
-      <c r="A37" s="3">
+        <v>32</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
         <v>4</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" ht="30">
+      <c r="B37" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>4</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>53</v>
+      <c r="B38" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>4</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>4</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>4</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
@@ -1249,14 +1325,20 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="7924580f-9edc-49cf-ad2d-ad0d5c68b011" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65872d6d-2405-4285-bf46-00301b302970">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005627606715B4514D89F36EED10136E48" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="8a4b3ca8819e3ffd5b98f54665cf41f4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65872d6d-2405-4285-bf46-00301b302970" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5746e54c2e4685cde5a4ca73fdde6a7d" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005627606715B4514D89F36EED10136E48" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3be56a7d6ff5f767b32100c8b7f531c9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65872d6d-2405-4285-bf46-00301b302970" xmlns:ns3="7924580f-9edc-49cf-ad2d-ad0d5c68b011" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b2d3130cdd2a31a35d41f9646d2cd5b" ns2:_="" ns3:_="">
     <xsd:import namespace="65872d6d-2405-4285-bf46-00301b302970"/>
+    <xsd:import namespace="7924580f-9edc-49cf-ad2d-ad0d5c68b011"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1266,6 +1348,13 @@
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1291,6 +1380,55 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0ef6089c-5148-4909-88ac-65974e5b7eb0" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7924580f-9edc-49cf-ad2d-ad0d5c68b011" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c69ace6f-2787-4afa-891b-b4e6d6b3e428}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7924580f-9edc-49cf-ad2d-ad0d5c68b011">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -1301,8 +1439,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1392,13 +1530,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95329DDE-5CC8-4797-9040-F970E31D22A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95329DDE-5CC8-4797-9040-F970E31D22A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BBB395C-07AF-439C-AD82-4CFF4E3B9B63}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BBB395C-07AF-439C-AD82-4CFF4E3B9B63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7924580f-9edc-49cf-ad2d-ad0d5c68b011"/>
+    <ds:schemaRef ds:uri="65872d6d-2405-4285-bf46-00301b302970"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AA2E0BF-E941-4EBD-8A73-537D21880863}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{249134CD-29CF-4CEE-A06A-085CBB61000D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="65872d6d-2405-4285-bf46-00301b302970"/>
+    <ds:schemaRef ds:uri="7924580f-9edc-49cf-ad2d-ad0d5c68b011"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>